<commit_message>
Financijski plan - završna verzija
</commit_message>
<xml_diff>
--- a/Obrazac za Financijski plan - tim 6.xlsx
+++ b/Obrazac za Financijski plan - tim 6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{132FC01B-C922-40E9-89E6-4241364892E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7016D6DD-9CA0-4465-B6F8-98D8CF32C6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Troškovi - Zaklada za xxxxxx</t>
   </si>
@@ -972,9 +972,6 @@
     <t>Trajanje projekta: od  01/01/2024  do  15/12/2024</t>
   </si>
   <si>
-    <t>Datum:  29.1.2023.</t>
-  </si>
-  <si>
     <t>3.1. Nova oprema</t>
   </si>
   <si>
@@ -992,15 +989,6 @@
     </r>
   </si>
   <si>
-    <t>3.1.4 Projektor</t>
-  </si>
-  <si>
-    <t>3.1.5 Platno</t>
-  </si>
-  <si>
-    <t>3.1.6 Bijela ploča s pomičnim postoljem</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Materijal, </t>
     </r>
@@ -1015,6 +1003,76 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">1.2.1 Tiskanje i slanje letaka osnovnim i srednjim školama (2000 kom.) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D1.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.7.1 Najam učionice (203,43 kn/sat, max 72 učenika)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> D1.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.3.2 Prijevoz 100 učenika i 3 člana projekta autobusom </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D2.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.3.2 Ručak (100 učenika + 3 člana projekta, 85 kn / osoba) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D2.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.1.2  500 listova A4 papira, 10 kom. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D1.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">1.1.1  Komplet dodatne opreme za bijelu ploču, 10 kom. </t>
     </r>
     <r>
@@ -1042,12 +1100,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>D1.2.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.1.2  500 listova A4 papira, 2 kom. </t>
+      <t>D1.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.2.3 Printanje certifikata učenika (100 učenika) </t>
     </r>
     <r>
       <rPr>
@@ -1056,12 +1114,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>STAVKA D1.2.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.1.3  Kemijske olovke, 30 kom </t>
+      <t>STAVKA D2.9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.1. Plaća predavačima (3 dana tjedno po 2 sata, 50 kn/sat, 20 tjedana) </t>
     </r>
     <r>
       <rPr>
@@ -1070,12 +1128,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>STAVKA D1.2.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.2.1 Tiskanje i slanje letaka osnovnim i srednjim školama (2000 kom.) </t>
+      <t>STAVKA D1.3, D2.2, D2.3, D2.4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.2.2 Google ads kampanja (1 god., budžet 2500 kn + upravljanje 1000kn) </t>
     </r>
     <r>
       <rPr>
@@ -1084,11 +1142,81 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>STAVKA D1.2.1</t>
-    </r>
-  </si>
-  <si>
-    <t>3.1.1  Laptop, 4 kom.</t>
+      <t>STAVKA D1.1</t>
+    </r>
+  </si>
+  <si>
+    <t>4.1.1 Algebra seminari(Organizacija nastave - moderno programiranje za učenike, video konferencije u nastavi, izrada multimedijskih sadržaja za nastavu i igrifikacija obrazovanja)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.1.2 Smještaj 4 predavača (7 noćenja + doručak, Hotel Jadran) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D2.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.1.3 Prijevoz 4 predavača (autobusna karta) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D2.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.1.4 Ručak i večera 4 predavača(7 dana, 200 kn/osoba/dan) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D2.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.1.5 Naknada za pohađanje (500 kn) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D2.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3.1.1  Laptop, 4 kom. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D1.2</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1100,29 +1228,16 @@
         <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>STAVKA D1.3.1</t>
-    </r>
-  </si>
-  <si>
-    <t>2.1. Plaća predavačima (3 dana tjedno po 2 sata, 45 kn/sat, 20 tjedana)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4.1.1 Smještaj 4 predavača (5 noćenja + doručak, Hotel Jadran) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
+      <t>STAVKA D2.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>STAVKA D1.2.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4.1.2 Prijevoz 4 predavača (autobusna karta) </t>
+      <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
@@ -1131,26 +1246,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>STAVKA D1.2.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4.1.3 Ručak i večera 4 predavača(5 dana, 150 kn/osoba/dan) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
+      <t>D2.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>STAVKA D1.2.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.2.2 Google ads kampanja (1 god., budžet 3125 kn + upravljanje 1500kn) </t>
+      <t>,</t>
     </r>
     <r>
       <rPr>
@@ -1159,15 +1264,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>STAVKA D1.2.1</t>
-    </r>
-  </si>
-  <si>
-    <t>4.7.1 Najam učionice (150 kn/sat, max 30 učenika)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.3.2 Prijevoz 100 učenika i 4 predavača autobusom </t>
+      <t xml:space="preserve"> D2.4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3.1.2 Projektor, 1 kom. </t>
     </r>
     <r>
       <rPr>
@@ -1176,12 +1278,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>STAVKA D2.1.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.3.2 Ručak (100 učenika + 4 predavača, 85 kn / osoba) </t>
+      <t>STAVKA D1.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.1.3  Kemijske olovke, 30 kom. </t>
     </r>
     <r>
       <rPr>
@@ -1190,8 +1292,57 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>STAVKA D2.1.1</t>
-    </r>
+      <t>STAVKA D1.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3.1.3 mBot2, 5 kom. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D1.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>D2.8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3.1.4 Programabilne pločice Arduino UNO Rev3, 10 kom. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>STAVKA D1.2, D2.8</t>
+    </r>
+  </si>
+  <si>
+    <t>Datum:  01.02.2023.</t>
   </si>
 </sst>
 </file>
@@ -1596,84 +1747,80 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="4" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1894,10 +2041,10 @@
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1909,12 +2056,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="55"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1925,36 +2072,36 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="44"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="44"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
+      <c r="A5" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
+      <c r="A6" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
@@ -1970,7 +2117,7 @@
     </row>
     <row r="8" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1978,11 +2125,11 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="44"/>
+        <v>55</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="55"/>
     </row>
     <row r="10" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1994,33 +2141,34 @@
     </row>
     <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" s="9">
-        <v>5643</v>
+        <v>2821.67</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9">
-        <f t="shared" ref="D10:D13" si="0">B11+C11</f>
-        <v>5643</v>
+        <f t="shared" ref="D11:D13" si="0">B11+C11</f>
+        <v>2821.67</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="9">
-        <v>119.8</v>
+        <f>59.9 * 10</f>
+        <v>599</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9">
         <f t="shared" si="0"/>
-        <v>119.8</v>
+        <v>599</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="68" t="s">
-        <v>62</v>
+      <c r="A13" s="50" t="s">
+        <v>73</v>
       </c>
       <c r="B13" s="9">
         <f xml:space="preserve"> 3.32 * 30</f>
@@ -2033,337 +2181,353 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="69"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="57"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="34"/>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="B15" s="59"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1145.24</v>
+      </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="59" t="s">
-        <v>63</v>
+      <c r="D17" s="9">
+        <f t="shared" ref="D17:D19" si="1">B17+C17</f>
+        <v>1145.24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="46" t="s">
+        <v>64</v>
       </c>
       <c r="B18" s="9">
-        <v>1145.24</v>
-      </c>
-      <c r="C18" s="9"/>
+        <f>3500 * 12</f>
+        <v>42000</v>
+      </c>
+      <c r="C18" s="48"/>
       <c r="D18" s="9">
-        <f t="shared" ref="D17:D19" si="1">B18+C18</f>
-        <v>1145.24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="59" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="9">
-        <f>4625 * 12</f>
-        <v>55500</v>
-      </c>
-      <c r="C19" s="64"/>
+        <f t="shared" si="1"/>
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="12">
+        <v>547.5</v>
+      </c>
+      <c r="C19" s="49"/>
       <c r="D19" s="9">
         <f t="shared" si="1"/>
-        <v>55500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="56"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+        <v>547.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="44"/>
-    </row>
-    <row r="22" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+      <c r="B20" s="59"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="55"/>
+    </row>
+    <row r="21" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9">
+        <f t="shared" ref="D21:D23" si="2">B21+C21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="9">
+        <f>22 * 103</f>
+        <v>2266</v>
+      </c>
+      <c r="C22" s="48"/>
       <c r="D22" s="9">
-        <f t="shared" ref="D22:D24" si="2">B22+C22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="9">
-        <f>22 * 104</f>
-        <v>2288</v>
-      </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="9">
         <f t="shared" si="2"/>
-        <v>2288</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="12">
-        <f xml:space="preserve"> 85 * 104</f>
-        <v>8840</v>
-      </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="56">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="12">
+        <f xml:space="preserve"> 85 * 103</f>
+        <v>8755</v>
+      </c>
+      <c r="C23" s="49"/>
+      <c r="D23" s="43">
         <f t="shared" si="2"/>
-        <v>8840</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+        <v>8755</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="44"/>
-    </row>
-    <row r="26" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
+      <c r="B24" s="59"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="55"/>
+    </row>
+    <row r="25" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="9">
-        <f>B26+C26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="56"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+      <c r="B25" s="42"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="43">
+        <f>B25+C25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="44"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+      <c r="B26" s="58"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="55"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9">
-        <f>B29+C29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9">
+        <f>B27+C27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="15">
-        <f t="shared" ref="B30:C30" si="3">SUM(B9:B29)</f>
-        <v>73635.64</v>
-      </c>
-      <c r="C30" s="15">
+      <c r="B28" s="15">
+        <f>SUM(B9:B27)</f>
+        <v>58234.01</v>
+      </c>
+      <c r="C28" s="15">
+        <f>SUM(C9:C27)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="15">
+        <f>SUM(D9:D27)</f>
+        <v>58234.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="61"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="55"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="9">
+        <f>50 * 2*2*3*20</f>
+        <v>12000</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9">
+        <f t="shared" ref="D31:D32" si="3">B31+C31</f>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="20"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D30" s="15">
-        <f>SUM(D9:D29)</f>
-        <v>73635.64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="18"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="49"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="44"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="9">
-        <f>45 * 2*2*3*20</f>
-        <v>10800</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9">
-        <f t="shared" ref="D33:D34" si="4">B33+C33</f>
-        <v>10800</v>
-      </c>
+      <c r="A33" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="60"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="55"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
+      <c r="A34" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9">
+        <f>B34+C34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="15">
+        <f t="shared" ref="B35:D35" si="4">SUM(B30:B34)</f>
+        <v>12000</v>
+      </c>
+      <c r="C35" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="42"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="44"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9">
-        <f>B36+C36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="15">
-        <f t="shared" ref="B37:D37" si="5">SUM(B32:B36)</f>
-        <v>10800</v>
-      </c>
-      <c r="C37" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D37" s="15">
-        <f t="shared" si="5"/>
-        <v>10800</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
+      <c r="D35" s="15">
+        <f t="shared" si="4"/>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="18"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="61"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="55"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="38"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="39"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="49"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="44"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="39"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" s="9">
+      <c r="A39" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="9">
         <f xml:space="preserve"> 4500*4</f>
         <v>18000</v>
       </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="9">
-        <f>B41+C41</f>
+      <c r="C39" s="48"/>
+      <c r="D39" s="9">
+        <f>B39+C39</f>
         <v>18000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="42">
+        <v>1394</v>
+      </c>
+      <c r="C40" s="49"/>
+      <c r="D40" s="43">
+        <f>C40+B40</f>
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="42">
+        <f xml:space="preserve"> 1500 *5</f>
+        <v>7500</v>
+      </c>
+      <c r="C41" s="49"/>
+      <c r="D41" s="43">
+        <f>C41+B41</f>
+        <v>7500</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="55">
-        <v>3504</v>
-      </c>
-      <c r="C42" s="65"/>
-      <c r="D42" s="56">
+        <v>75</v>
+      </c>
+      <c r="B42" s="42">
+        <f>279*10</f>
+        <v>2790</v>
+      </c>
+      <c r="C42" s="49"/>
+      <c r="D42" s="43">
         <f>C42+B42</f>
-        <v>3504</v>
+        <v>2790</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="55">
-        <v>1000</v>
-      </c>
-      <c r="C43" s="65"/>
-      <c r="D43" s="56">
-        <f t="shared" ref="D43:D44" si="6">C43+B43</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="55">
-        <v>2403</v>
-      </c>
-      <c r="C44" s="65"/>
-      <c r="D44" s="56">
-        <f t="shared" si="6"/>
-        <v>2403</v>
+      <c r="A43" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="65"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="67"/>
+    </row>
+    <row r="44" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9">
+        <f>B44+C44</f>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="66"/>
-      <c r="D45" s="51"/>
-    </row>
-    <row r="46" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="B45" s="60"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="55"/>
+    </row>
+    <row r="46" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="23" t="s">
+        <v>24</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
@@ -2372,118 +2536,126 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="42"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="44"/>
-    </row>
-    <row r="48" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9">
-        <f>B48+C48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="14" t="s">
+    <row r="47" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="15">
-        <f>SUM(B39:B48)</f>
-        <v>24907</v>
-      </c>
-      <c r="C49" s="15">
-        <f>SUM(C39:C48)</f>
-        <v>0</v>
-      </c>
-      <c r="D49" s="15">
-        <f>SUM(D39:D48)</f>
-        <v>24907</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="16" t="s">
+      <c r="B47" s="15">
+        <f>SUM(B37:B46)</f>
+        <v>29684</v>
+      </c>
+      <c r="C47" s="15">
+        <f>SUM(C37:C46)</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="15">
+        <f>SUM(D37:D46)</f>
+        <v>29684</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="18"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="19" t="s">
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="18"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="49"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="44"/>
-    </row>
-    <row r="52" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="8" t="s">
+      <c r="B49" s="61"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="55"/>
+    </row>
+    <row r="50" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="9">
+      <c r="B50" s="9"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="9">
+        <f>B50+C50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="42">
+        <f>32*95*4</f>
+        <v>12160</v>
+      </c>
+      <c r="C51" s="49"/>
+      <c r="D51" s="9">
+        <f>B51+C51</f>
+        <v>12160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="42">
+        <f xml:space="preserve"> 1400 * 7</f>
+        <v>9800</v>
+      </c>
+      <c r="C52" s="49"/>
+      <c r="D52" s="43">
         <f>B52+C52</f>
-        <v>0</v>
+        <v>9800</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="58" t="s">
+      <c r="A53" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="55">
-        <f xml:space="preserve"> 1400 * 5</f>
-        <v>7000</v>
-      </c>
-      <c r="C53" s="65"/>
-      <c r="D53" s="56">
-        <f>B53+C53</f>
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="B54" s="55">
+      <c r="B53" s="42">
         <f xml:space="preserve"> 67.5 * 2 * 4</f>
         <v>540</v>
       </c>
-      <c r="C54" s="65"/>
-      <c r="D54" s="56">
+      <c r="C53" s="49"/>
+      <c r="D53" s="43">
+        <f>B53+C53</f>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="42">
+        <f xml:space="preserve"> 200 * 4 * 7</f>
+        <v>5600</v>
+      </c>
+      <c r="C54" s="49"/>
+      <c r="D54" s="43">
         <f>B54+C54</f>
-        <v>540</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="58" t="s">
+      <c r="A55" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="55">
-        <f xml:space="preserve"> 150 * 4 * 5</f>
-        <v>3000</v>
-      </c>
-      <c r="C55" s="65"/>
-      <c r="D55" s="56">
+      <c r="B55" s="42">
+        <v>2000</v>
+      </c>
+      <c r="C55" s="49"/>
+      <c r="D55" s="43">
         <f>B55+C55</f>
-        <v>3000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B56" s="42"/>
-      <c r="C56" s="67"/>
-      <c r="D56" s="44"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="55"/>
     </row>
     <row r="57" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
@@ -2492,7 +2664,7 @@
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9">
-        <f t="shared" ref="D57:D61" si="7">B57+C57</f>
+        <f t="shared" ref="D57:D61" si="5">B57+C57</f>
         <v>0</v>
       </c>
     </row>
@@ -2503,7 +2675,7 @@
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2514,7 +2686,7 @@
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2523,7 +2695,7 @@
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2532,7 +2704,7 @@
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2540,9 +2712,9 @@
       <c r="A62" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B62" s="42"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="44"/>
+      <c r="B62" s="60"/>
+      <c r="C62" s="54"/>
+      <c r="D62" s="55"/>
     </row>
     <row r="63" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
@@ -2551,20 +2723,20 @@
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9">
-        <f t="shared" ref="D63:D64" si="8">B63+C63</f>
+        <f t="shared" ref="D63:D64" si="6">B63+C63</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="36" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B64" s="9">
         <v>1425</v>
       </c>
       <c r="C64" s="9"/>
       <c r="D64" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1425</v>
       </c>
     </row>
@@ -2578,9 +2750,9 @@
       <c r="A66" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="42"/>
-      <c r="C66" s="43"/>
-      <c r="D66" s="44"/>
+      <c r="B66" s="60"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="55"/>
     </row>
     <row r="67" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="23" t="s">
@@ -2589,7 +2761,7 @@
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
       <c r="D67" s="9">
-        <f t="shared" ref="D67:D75" si="9">B67+C67</f>
+        <f t="shared" ref="D67:D75" si="7">B67+C67</f>
         <v>0</v>
       </c>
     </row>
@@ -2598,7 +2770,7 @@
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2607,7 +2779,7 @@
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2616,7 +2788,7 @@
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2627,7 +2799,7 @@
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2636,7 +2808,7 @@
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2647,7 +2819,7 @@
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
       <c r="D73" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2656,7 +2828,7 @@
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2665,7 +2837,7 @@
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
       <c r="D75" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2690,22 +2862,22 @@
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="9">
-        <f t="shared" ref="D78:D80" si="10">B78+C78</f>
+        <f t="shared" ref="D78:D80" si="8">B78+C78</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="36" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B79" s="9">
-        <f>150*2*3*20</f>
-        <v>18000</v>
+        <f>203.43*2*3*20</f>
+        <v>24411.599999999999</v>
       </c>
       <c r="C79" s="9"/>
       <c r="D79" s="9">
-        <f t="shared" si="10"/>
-        <v>18000</v>
+        <f t="shared" si="8"/>
+        <v>24411.599999999999</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2715,28 +2887,28 @@
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
       <c r="D80" s="9">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B81" s="15">
-        <f t="shared" ref="B81:D81" si="11">SUM(B51:B80)</f>
-        <v>29965</v>
+        <f t="shared" ref="B81:C81" si="9">SUM(B49:B80)</f>
+        <v>55936.6</v>
       </c>
       <c r="C81" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="D81" s="15">
-        <f>SUM(D51:D80)</f>
-        <v>29965</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <f>SUM(D49:D80)</f>
+        <v>55936.6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="16" t="s">
         <v>43</v>
       </c>
@@ -2744,7 +2916,7 @@
       <c r="C82" s="17"/>
       <c r="D82" s="18"/>
     </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
         <v>44</v>
       </c>
@@ -2755,47 +2927,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="8"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="27"/>
     </row>
-    <row r="85" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
         <v>45</v>
       </c>
       <c r="B85" s="15">
-        <f t="shared" ref="B85:D85" si="12">SUM(B83:B84)</f>
+        <f t="shared" ref="B85:D85" si="10">SUM(B83:B84)</f>
         <v>0</v>
       </c>
       <c r="C85" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D85" s="15">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B86" s="15">
-        <f>B30+B37+B49+B81+B85</f>
-        <v>139307.64000000001</v>
+        <f>B28+B35+B47+B81+B85</f>
+        <v>155854.61000000002</v>
       </c>
       <c r="C86" s="15">
-        <f>C30+C37+C49+C81+C85</f>
+        <f>C28+C35+C47+C81+C85</f>
         <v>0</v>
       </c>
       <c r="D86" s="15">
-        <f>D30+D37+D49+D81+D85</f>
-        <v>139307.64000000001</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <f>D28+D35+D47+D81+D85</f>
+        <v>155854.61000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="28" t="s">
         <v>47</v>
       </c>
@@ -2803,48 +2975,49 @@
       <c r="C87" s="15"/>
       <c r="D87" s="15"/>
     </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="29"/>
       <c r="B88" s="30"/>
       <c r="C88" s="30"/>
       <c r="D88" s="31"/>
     </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="32"/>
       <c r="B89" s="30"/>
       <c r="C89" s="30"/>
       <c r="D89" s="33"/>
-    </row>
-    <row r="90" spans="1:4" ht="171" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="45" t="s">
+      <c r="E89" s="69"/>
+    </row>
+    <row r="90" spans="1:5" ht="171" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="B90" s="46"/>
-      <c r="C90" s="46"/>
-      <c r="D90" s="46"/>
+      <c r="B90" s="64"/>
+      <c r="C90" s="64"/>
+      <c r="D90" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B56:D56"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B45:D45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" cellComments="atEnd" r:id="rId1"/>

</xml_diff>